<commit_message>
feat(registro_de_asistencias): add test bot and sync excel data
</commit_message>
<xml_diff>
--- a/registro_de_asistencias/Reporte_SVC.xlsx
+++ b/registro_de_asistencias/Reporte_SVC.xlsx
@@ -7,22 +7,188 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId1" sheetId="1" name="Jugadores"/>
+    <sheet r:id="rId2" sheetId="2" name="Asistencias"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
+  <si>
+    <t>ID</t>
+  </si>
   <si>
     <t>Jugador</t>
   </si>
   <si>
+    <t>Codigo</t>
+  </si>
+  <si>
     <t>Fecha</t>
   </si>
   <si>
     <t>Hora</t>
+  </si>
+  <si>
+    <t>Nicolas Pereira</t>
+  </si>
+  <si>
+    <t>6607</t>
+  </si>
+  <si>
+    <t>2026-02-18</t>
+  </si>
+  <si>
+    <t>01:08</t>
+  </si>
+  <si>
+    <t>01:07</t>
+  </si>
+  <si>
+    <t>Juan Gonzales</t>
+  </si>
+  <si>
+    <t>2563</t>
+  </si>
+  <si>
+    <t>00:42</t>
+  </si>
+  <si>
+    <t>Ishar Pereyra</t>
+  </si>
+  <si>
+    <t>7745</t>
+  </si>
+  <si>
+    <t>Iganacio Cabrera</t>
+  </si>
+  <si>
+    <t>6749</t>
+  </si>
+  <si>
+    <t>00:41</t>
+  </si>
+  <si>
+    <t>Juan Machado</t>
+  </si>
+  <si>
+    <t>6117</t>
+  </si>
+  <si>
+    <t>Ignacio Machado</t>
+  </si>
+  <si>
+    <t>8574</t>
+  </si>
+  <si>
+    <t>00:40</t>
+  </si>
+  <si>
+    <t>Julio Cabrera</t>
+  </si>
+  <si>
+    <t>8029</t>
+  </si>
+  <si>
+    <t>00:39</t>
+  </si>
+  <si>
+    <t>00:38</t>
+  </si>
+  <si>
+    <t>00:37</t>
+  </si>
+  <si>
+    <t>00:34</t>
+  </si>
+  <si>
+    <t>Akumi de Prueba</t>
+  </si>
+  <si>
+    <t>2468</t>
+  </si>
+  <si>
+    <t>2026-02-17</t>
+  </si>
+  <si>
+    <t>23:59</t>
+  </si>
+  <si>
+    <t>23:15</t>
+  </si>
+  <si>
+    <t>23:09</t>
+  </si>
+  <si>
+    <t>23:02</t>
+  </si>
+  <si>
+    <t>23:01</t>
+  </si>
+  <si>
+    <t>Edad</t>
+  </si>
+  <si>
+    <t>Tiempo</t>
+  </si>
+  <si>
+    <t>Nicolás Pereira — 20</t>
+  </si>
+  <si>
+    <t>Ignacio Cabrera — 19</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Nahuel Navas — 21</t>
+  </si>
+  <si>
+    <t>Julio Cabrera — 18</t>
+  </si>
+  <si>
+    <t>Ishar Pereyra — 17</t>
+  </si>
+  <si>
+    <t>Juan Ferreyra — 18</t>
+  </si>
+  <si>
+    <t>Joaquín Juvencio — 21</t>
+  </si>
+  <si>
+    <t>Kevin Barreto — 25</t>
+  </si>
+  <si>
+    <t>Matías Martinez — 37</t>
+  </si>
+  <si>
+    <t>7911</t>
+  </si>
+  <si>
+    <t>Facundo Carrión — 17</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>Joaquín Cordero — 20</t>
+  </si>
+  <si>
+    <t>6991</t>
+  </si>
+  <si>
+    <t>Manuel Rocha — 25</t>
+  </si>
+  <si>
+    <t>2624</t>
+  </si>
+  <si>
+    <t>Juan Gonzáles — 30</t>
+  </si>
+  <si>
+    <t>5323</t>
   </si>
 </sst>
 </file>
@@ -30,13 +196,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,7 +219,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -59,12 +238,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -369,26 +563,860 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1423</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6">
+        <v>8029</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="3"/>
+      <c r="B9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>8574</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3"/>
+      <c r="B11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2563</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3"/>
+      <c r="B15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="3">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="6">
+        <v>4574</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="3">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="3">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3">
+        <v>19</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3">
+        <v>21</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="3">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3">
+        <v>23</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="3">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3">
+        <v>25</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="3">
+        <v>30</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="3">
+        <v>27</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="3">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="3">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="3">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>